<commit_message>
added excel of time line
added time line
</commit_message>
<xml_diff>
--- a/Team_10_EEE3099S_Timeline.xlsx
+++ b/Team_10_EEE3099S_Timeline.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pilla\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/frskia001_myuct_ac_za/Documents/Desktop/uct/3 year/second semester/99/EEE3099S_CKT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26495B91-49CD-4D79-B21F-13BEFF98B5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="8_{26495B91-49CD-4D79-B21F-13BEFF98B5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D897AC59-CD84-4ABB-B8F5-AA33A80DABEA}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="3420" windowWidth="21600" windowHeight="11295" xr2:uid="{0EA59903-2EF2-4FC3-A659-A268362FD0C7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0EA59903-2EF2-4FC3-A659-A268362FD0C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,149 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>Week 11</t>
+  </si>
+  <si>
+    <t>Week 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task </t>
+  </si>
+  <si>
+    <t>VAC</t>
+  </si>
+  <si>
+    <t>person in charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction &amp; Req. Analysis   </t>
+  </si>
+  <si>
+    <t>Subsystem Design  </t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>Kian</t>
+  </si>
+  <si>
+    <t>ATP  </t>
+  </si>
+  <si>
+    <t>Thiyashan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timeline and PM Page  </t>
+  </si>
+  <si>
+    <t>Kian, Thiyashan</t>
+  </si>
+  <si>
+    <t>Onramp courses</t>
+  </si>
+  <si>
+    <t>weekly review</t>
+  </si>
+  <si>
+    <t>block diagram</t>
+  </si>
+  <si>
+    <t>references</t>
+  </si>
+  <si>
+    <t>milestone 2:</t>
+  </si>
+  <si>
+    <t>milestone 1:</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Report:</t>
+  </si>
+  <si>
+    <t>Distance and Angle Control Algorithm</t>
+  </si>
+  <si>
+    <t>Line following algorithm</t>
+  </si>
+  <si>
+    <t>Object Detection Algorithm</t>
+  </si>
+  <si>
+    <t>Localisation Algorithm</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demo: </t>
+  </si>
+  <si>
+    <t>MATLAB code:</t>
+  </si>
+  <si>
+    <t>Camaron</t>
+  </si>
+  <si>
+    <t>milestone 3</t>
+  </si>
+  <si>
+    <t>milestone 4</t>
+  </si>
+  <si>
+    <t>finale report:</t>
+  </si>
+  <si>
+    <t>The hunt:</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +185,102 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -62,12 +288,273 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,12 +869,532 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02124F0-C5F8-40BE-AC60-865812D3D94F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="21">
+        <v>45131</v>
+      </c>
+      <c r="E2" s="21">
+        <v>45138</v>
+      </c>
+      <c r="F2" s="21">
+        <v>45145</v>
+      </c>
+      <c r="G2" s="21">
+        <v>45152</v>
+      </c>
+      <c r="H2" s="21">
+        <v>45159</v>
+      </c>
+      <c r="I2" s="21">
+        <v>45166</v>
+      </c>
+      <c r="J2" s="21">
+        <v>45173</v>
+      </c>
+      <c r="K2" s="21">
+        <v>45180</v>
+      </c>
+      <c r="L2" s="21">
+        <v>45187</v>
+      </c>
+      <c r="M2" s="21">
+        <v>45194</v>
+      </c>
+      <c r="N2" s="21">
+        <v>45201</v>
+      </c>
+      <c r="O2" s="21">
+        <v>45208</v>
+      </c>
+      <c r="P2" s="22">
+        <v>45215</v>
+      </c>
+      <c r="Q2" s="17"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="17"/>
+    </row>
+    <row r="4" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="17"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="27"/>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="2"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="17"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="27"/>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="17"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="27"/>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="2"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="17"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="27"/>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="5"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="17"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="27"/>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="17"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="27"/>
+      <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="17"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="27"/>
+      <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="2"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="17"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="28"/>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="5"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="17"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="29"/>
+      <c r="B13" s="3"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="17"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="29"/>
+      <c r="B14" s="3"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="17"/>
+    </row>
+    <row r="15" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="11"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="17"/>
+    </row>
+    <row r="16" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="27"/>
+      <c r="B16" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="17"/>
+    </row>
+    <row r="17" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="27"/>
+      <c r="B17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="17"/>
+    </row>
+    <row r="18" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27"/>
+      <c r="B18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="17"/>
+    </row>
+    <row r="19" spans="1:17" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="27"/>
+      <c r="B19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="17"/>
+    </row>
+    <row r="20" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27"/>
+      <c r="B20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="17"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="27"/>
+      <c r="B21" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K21" s="9"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="17"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="27"/>
+      <c r="B22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="17"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="28"/>
+      <c r="B23" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="17"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="29"/>
+      <c r="B24" s="3"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="17"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="29"/>
+      <c r="B25" s="3"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="17"/>
+    </row>
+    <row r="26" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="17"/>
+    </row>
+    <row r="27" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="27"/>
+      <c r="B27" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="17"/>
+    </row>
+    <row r="28" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="31"/>
+      <c r="B28" s="3"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="17"/>
+    </row>
+    <row r="29" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="31"/>
+      <c r="B29" s="3"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="17"/>
+    </row>
+    <row r="30" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P30" s="32"/>
+      <c r="Q30" s="17"/>
+    </row>
+    <row r="31" spans="1:17" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="33"/>
+      <c r="B31" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="34"/>
+      <c r="O31" s="34"/>
+      <c r="P31" s="35"/>
+      <c r="Q31" s="17"/>
+    </row>
+    <row r="32" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+    </row>
+    <row r="33" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="16"/>
+    </row>
+    <row r="34" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="16"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="A15:A23"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A30:A31"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>